<commit_message>
Commit with Precision Recall Plot and the final results to an Excel.
</commit_message>
<xml_diff>
--- a/Code/Portuguese_Bank_Marketing_Project/results_final.xlsx
+++ b/Code/Portuguese_Bank_Marketing_Project/results_final.xlsx
@@ -58,22 +58,22 @@
     <t>Random Forest</t>
   </si>
   <si>
+    <t>Decision Tree</t>
+  </si>
+  <si>
     <t>Logistic Regression</t>
   </si>
   <si>
-    <t>Decision Tree</t>
-  </si>
-  <si>
     <t>Gaussian Naive-Bayes</t>
   </si>
   <si>
     <t>Bernoulli Naive-Bayes</t>
   </si>
   <si>
+    <t>Reduced</t>
+  </si>
+  <si>
     <t>Full</t>
-  </si>
-  <si>
-    <t>Reduced</t>
   </si>
   <si>
     <t>Default</t>
@@ -495,77 +495,77 @@
         <v>20</v>
       </c>
       <c r="E2">
-        <v>0.9479985972646661</v>
+        <v>0.9468463503832474</v>
       </c>
       <c r="F2">
-        <v>0.9458945894589459</v>
+        <v>0.9423942394239424</v>
       </c>
       <c r="G2">
-        <v>0.9500753390256153</v>
+        <v>0.9510496568429552</v>
       </c>
       <c r="H2">
-        <v>0.9906508518749887</v>
+        <v>0.9910657197018637</v>
       </c>
       <c r="I2">
-        <v>9458</v>
+        <v>9423</v>
       </c>
       <c r="J2">
-        <v>9465</v>
+        <v>9477</v>
       </c>
       <c r="K2">
-        <v>497</v>
+        <v>485</v>
       </c>
       <c r="L2">
-        <v>541</v>
+        <v>576</v>
       </c>
       <c r="M2">
-        <v>275470</v>
+        <v>292850</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3">
-        <v>0.9436901958819699</v>
+        <v>0.9469966434547368</v>
       </c>
       <c r="F3">
-        <v>0.9666966696669667</v>
+        <v>0.9681968196819682</v>
       </c>
       <c r="G3">
-        <v>0.9243568901214497</v>
+        <v>0.9289895403512139</v>
       </c>
       <c r="H3">
-        <v>0.9898487539980659</v>
+        <v>0.9908716278172688</v>
       </c>
       <c r="I3">
-        <v>9666</v>
+        <v>9681</v>
       </c>
       <c r="J3">
-        <v>9171</v>
+        <v>9222</v>
       </c>
       <c r="K3">
-        <v>791</v>
+        <v>740</v>
       </c>
       <c r="L3">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="M3">
-        <v>174410</v>
+        <v>166400</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
@@ -574,34 +574,34 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4">
-        <v>0.8568708982515906</v>
+        <v>0.8570712890135764</v>
       </c>
       <c r="F4">
-        <v>0.858085808580858</v>
+        <v>0.8905890589058906</v>
       </c>
       <c r="G4">
-        <v>0.8564583749251348</v>
+        <v>0.8350525131282821</v>
       </c>
       <c r="H4">
-        <v>0.9250213818812115</v>
+        <v>0.9347231601297051</v>
       </c>
       <c r="I4">
-        <v>8580</v>
+        <v>8905</v>
       </c>
       <c r="J4">
-        <v>8524</v>
+        <v>8203</v>
       </c>
       <c r="K4">
-        <v>1438</v>
+        <v>1759</v>
       </c>
       <c r="L4">
-        <v>1419</v>
+        <v>1094</v>
       </c>
       <c r="M4">
-        <v>723880</v>
+        <v>564590</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -612,119 +612,119 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
       </c>
       <c r="E5">
-        <v>0.9034116527228094</v>
+        <v>0.8232553479284604</v>
       </c>
       <c r="F5">
-        <v>0.9082908290829083</v>
+        <v>0.8277827782778278</v>
       </c>
       <c r="G5">
-        <v>0.8998315664321808</v>
+        <v>0.8208866408806903</v>
       </c>
       <c r="H5">
-        <v>0.9034025918150939</v>
+        <v>0.8929961456294193</v>
       </c>
       <c r="I5">
-        <v>9082</v>
+        <v>8277</v>
       </c>
       <c r="J5">
-        <v>8951</v>
+        <v>8156</v>
       </c>
       <c r="K5">
-        <v>1011</v>
+        <v>1806</v>
       </c>
       <c r="L5">
-        <v>917</v>
+        <v>1722</v>
       </c>
       <c r="M5">
-        <v>468610</v>
+        <v>879060</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
       <c r="E6">
-        <v>0.7198036170532538</v>
+        <v>0.7034717699514053</v>
       </c>
       <c r="F6">
-        <v>0.5614561456145615</v>
+        <v>0.8596859685968596</v>
       </c>
       <c r="G6">
-        <v>0.8229258282028731</v>
+        <v>0.6555826723611958</v>
       </c>
       <c r="H6">
-        <v>0.8163541208567754</v>
+        <v>0.8058707296146197</v>
       </c>
       <c r="I6">
-        <v>5614</v>
+        <v>8596</v>
       </c>
       <c r="J6">
-        <v>8754</v>
+        <v>5446</v>
       </c>
       <c r="K6">
-        <v>1208</v>
+        <v>4516</v>
       </c>
       <c r="L6">
-        <v>4385</v>
+        <v>1403</v>
       </c>
       <c r="M6">
-        <v>2204580</v>
+        <v>746660</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
       </c>
       <c r="E7">
-        <v>0.6651470367216071</v>
+        <v>0.6491658734532338</v>
       </c>
       <c r="F7">
-        <v>0.6018601860186018</v>
+        <v>0.6465646564656465</v>
       </c>
       <c r="G7">
-        <v>0.6900584795321637</v>
+        <v>0.6507952486410308</v>
       </c>
       <c r="H7">
-        <v>0.7320789647726066</v>
+        <v>0.7062773432532974</v>
       </c>
       <c r="I7">
-        <v>6018</v>
+        <v>6465</v>
       </c>
       <c r="J7">
-        <v>7259</v>
+        <v>6493</v>
       </c>
       <c r="K7">
-        <v>2703</v>
+        <v>3469</v>
       </c>
       <c r="L7">
-        <v>3981</v>
+        <v>3534</v>
       </c>
       <c r="M7">
-        <v>2017530</v>
+        <v>1801690</v>
       </c>
     </row>
   </sheetData>

</xml_diff>